<commit_message>
fix problems on std files
</commit_message>
<xml_diff>
--- a/standard_formats/fishglob_data_columns_std.xlsx
+++ b/standard_formats/fishglob_data_columns_std.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/auroremaureaud/Documents/FISHGLOB/integrated_fishglob_surveys/standard_formats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F25AE55D-5B0B-8E45-8110-BF9098BB0516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5311FE17-0749-A848-A641-9C55EE6D8870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-6420" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{A578349E-914C-4F40-B01E-02B84B84F444}"/>
   </bookViews>
@@ -336,21 +336,6 @@
     <t>combination of survey with quarter or season (useful for BITS, NS-IBTS, SWC-IBTS, NEUS, SEUS, SCS)</t>
   </si>
   <si>
-    <t>trimming_hex7_0</t>
-  </si>
-  <si>
-    <t>trimming_hex7_2</t>
-  </si>
-  <si>
-    <t>trimming_hex8_0</t>
-  </si>
-  <si>
-    <t>trimming_hex8_2</t>
-  </si>
-  <si>
-    <t>trimming_biotime</t>
-  </si>
-  <si>
     <t>TRUE/FALSE, TRUE if haul should be kept, FALSE if haul should be removed</t>
   </si>
   <si>
@@ -376,6 +361,21 @@
   </si>
   <si>
     <t>wgt_cpua</t>
+  </si>
+  <si>
+    <t>flag_trimming_hex7_0</t>
+  </si>
+  <si>
+    <t>flag_trimming_hex7_2</t>
+  </si>
+  <si>
+    <t>flag_trimming_hex8_0</t>
+  </si>
+  <si>
+    <t>flag_trimming_hex8_2</t>
+  </si>
+  <si>
+    <t>flag_trimming_2</t>
   </si>
 </sst>
 </file>
@@ -442,7 +442,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -730,7 +730,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -740,8 +740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBE071AB-EC29-4233-A8DC-D691A27387F7}">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -779,26 +779,26 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1072,7 +1072,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B27" t="s">
         <v>61</v>
@@ -1114,7 +1114,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B30" t="s">
         <v>69</v>
@@ -1271,68 +1271,68 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
+        <v>106</v>
+      </c>
+      <c r="C44" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44" t="s">
         <v>97</v>
-      </c>
-      <c r="C44" t="s">
-        <v>5</v>
-      </c>
-      <c r="D44" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="C45" t="s">
         <v>5</v>
       </c>
       <c r="D45" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="C46" t="s">
         <v>5</v>
       </c>
       <c r="D46" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="C47" t="s">
         <v>5</v>
       </c>
       <c r="D47" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="C48" t="s">
         <v>5</v>
       </c>
       <c r="D48" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C49" t="s">
         <v>5</v>
       </c>
       <c r="D49" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
include readme file to write Rdatafiles
</commit_message>
<xml_diff>
--- a/standard_formats/fishglob_data_columns_std.xlsx
+++ b/standard_formats/fishglob_data_columns_std.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/auroremaureaud/Documents/FISHGLOB/integrated_fishglob_surveys/standard_formats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5311FE17-0749-A848-A641-9C55EE6D8870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25774560-6FFB-1442-82A7-9889B45150EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-6420" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{A578349E-914C-4F40-B01E-02B84B84F444}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="110">
   <si>
     <t>Column name fishglob</t>
   </si>
@@ -333,18 +333,9 @@
     <t>survey_unit</t>
   </si>
   <si>
-    <t>combination of survey with quarter or season (useful for BITS, NS-IBTS, SWC-IBTS, NEUS, SEUS, SCS)</t>
-  </si>
-  <si>
-    <t>TRUE/FALSE, TRUE if haul should be kept, FALSE if haul should be removed</t>
-  </si>
-  <si>
     <t>flag_taxa</t>
   </si>
   <si>
-    <t>TRUE/FALSE, TRUE if taxa should be kept, FALSE if taxa should be removed</t>
-  </si>
-  <si>
     <t>source</t>
   </si>
   <si>
@@ -376,6 +367,12 @@
   </si>
   <si>
     <t>flag_trimming_2</t>
+  </si>
+  <si>
+    <t>TRUE if haul is flagged, NA if not</t>
+  </si>
+  <si>
+    <t>combination of survey with quarter or season (useful for BITS, NS-IBTS, SWC-IBTS, NEUS, SEUS, SCS, GMEX)</t>
   </si>
 </sst>
 </file>
@@ -741,7 +738,7 @@
   <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -779,26 +776,26 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1072,7 +1069,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B27" t="s">
         <v>61</v>
@@ -1114,7 +1111,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B30" t="s">
         <v>69</v>
@@ -1266,73 +1263,73 @@
         <v>5</v>
       </c>
       <c r="D43" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C44" t="s">
         <v>5</v>
       </c>
       <c r="D44" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C45" t="s">
         <v>5</v>
       </c>
       <c r="D45" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
+        <v>105</v>
+      </c>
+      <c r="C46" t="s">
+        <v>5</v>
+      </c>
+      <c r="D46" t="s">
         <v>108</v>
-      </c>
-      <c r="C46" t="s">
-        <v>5</v>
-      </c>
-      <c r="D46" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C47" t="s">
         <v>5</v>
       </c>
       <c r="D47" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C48" t="s">
         <v>5</v>
       </c>
       <c r="D48" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C49" t="s">
         <v>5</v>
       </c>
       <c r="D49" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>